<commit_message>
diagramme de cas d'utilisation de recrutement et de départ
</commit_message>
<xml_diff>
--- a/Rapport stage/models/diagrammes.xlsx
+++ b/Rapport stage/models/diagrammes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFORMATIQUE\Cours\CEFIVE\Projet-Prof\Rapport stage\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INFORMATIQUE\Cours\CEFIVE\Projet-Prof\CEFIVE-Rapport-ProjetProf\Rapport stage\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6064,8 +6064,8 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
@@ -6080,8 +6080,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4343400" y="807720"/>
-          <a:ext cx="4008120" cy="5417820"/>
+          <a:off x="4343400" y="541020"/>
+          <a:ext cx="4008120" cy="5684520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6118,14 +6118,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>444622</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>138395</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>24094</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>263180</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>133201</xdr:rowOff>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6134,8 +6134,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5199502" y="869915"/>
-          <a:ext cx="2195998" cy="360566"/>
+          <a:off x="5199502" y="389854"/>
+          <a:ext cx="2195998" cy="859825"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -6894,8 +6894,8 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>519437</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>135798</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>88247</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
@@ -6913,8 +6913,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="2896877" y="1050198"/>
-          <a:ext cx="2302625" cy="1151283"/>
+          <a:off x="2896877" y="819767"/>
+          <a:ext cx="2302625" cy="1381714"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -8972,8 +8972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>